<commit_message>
Add Upper Monitor Offline Protocol
</commit_message>
<xml_diff>
--- a/Protocol_NeodAnderjon.xlsx
+++ b/Protocol_NeodAnderjon.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96412552-05A0-4132-8DD0-3E5D88D35AAF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF583F35-464D-4A6C-95CA-079FA27E72C8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>AA</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1103,6 +1103,38 @@
         <family val="3"/>
       </rPr>
       <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>正转</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>反转</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1505,7 +1537,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1770,36 +1802,36 @@
     </row>
     <row r="18" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>